<commit_message>
Various improvements to side-data
</commit_message>
<xml_diff>
--- a/tabular/references/hhv-ncbi-refseqs-side-data.xlsx
+++ b/tabular/references/hhv-ncbi-refseqs-side-data.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/general/HHV6-GLUE/tabular/references/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2E667D-72EA-564F-9BE3-EA92E1F36011}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1040" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REFSET" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,336 +25,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
-    <t>accession-ID</t>
+    <t>sequenceID</t>
   </si>
   <si>
-    <t>virus_name</t>
+    <t>NC_001664</t>
   </si>
   <si>
-    <t>virus_subfamily</t>
+    <t>NC_000898</t>
   </si>
   <si>
-    <t>virus_genus</t>
+    <t>exogenous</t>
   </si>
   <si>
-    <t>Parvovirinae</t>
+    <t>clade</t>
   </si>
   <si>
-    <t>Dependoparvovirus</t>
+    <t>gb_lab_construct</t>
   </si>
   <si>
-    <t>NC_001401</t>
+    <t>A1</t>
   </si>
   <si>
-    <t>AAV2</t>
+    <t>Uganda</t>
   </si>
   <si>
-    <t>NC_006148</t>
+    <t>country</t>
   </si>
   <si>
-    <t>DQ335246</t>
+    <t>U1102</t>
   </si>
   <si>
-    <t>CAV</t>
+    <t>Democratic Repuclic of Congo</t>
   </si>
   <si>
-    <t>NC_001701</t>
+    <t>Z29</t>
   </si>
   <si>
-    <t>GPV</t>
+    <t>locus</t>
   </si>
   <si>
-    <t>NC_006147</t>
+    <t>collection_year</t>
   </si>
   <si>
-    <t>MDPV</t>
+    <t>host_sci_name</t>
   </si>
   <si>
-    <t>Adeno-associated virus 2</t>
-  </si>
-  <si>
-    <t>Caprine adeno-associated virus</t>
-  </si>
-  <si>
-    <t>Goose parvovirus</t>
-  </si>
-  <si>
-    <t>Snake parvovirus 1</t>
-  </si>
-  <si>
-    <t>Muscovy duck parvovirus</t>
-  </si>
-  <si>
-    <t>virus_full_name</t>
-  </si>
-  <si>
-    <t>SnakePV</t>
-  </si>
-  <si>
-    <t>Mus musculus</t>
+    <t>NULL</t>
   </si>
   <si>
     <t>Homo sapiens</t>
   </si>
   <si>
-    <t>host_species</t>
-  </si>
-  <si>
-    <t>Capra hircus</t>
-  </si>
-  <si>
-    <t>Macaca mulatta</t>
-  </si>
-  <si>
-    <t>AF028704</t>
-  </si>
-  <si>
-    <t>AF028705</t>
-  </si>
-  <si>
-    <t>AX753250</t>
-  </si>
-  <si>
-    <t>AY243002</t>
-  </si>
-  <si>
-    <t>AY243021</t>
-  </si>
-  <si>
-    <t>AY243022</t>
-  </si>
-  <si>
-    <t>AY631966</t>
-  </si>
-  <si>
-    <t>DQ813647</t>
-  </si>
-  <si>
-    <t>KT984498</t>
-  </si>
-  <si>
-    <t>LY408697</t>
-  </si>
-  <si>
-    <t>NC_001729</t>
-  </si>
-  <si>
-    <t>NC_001829</t>
-  </si>
-  <si>
-    <t>NC_002077</t>
-  </si>
-  <si>
-    <t>NC_006152</t>
-  </si>
-  <si>
-    <t>NC_006260</t>
-  </si>
-  <si>
-    <t>NC_006261</t>
-  </si>
-  <si>
-    <t>NC_027429</t>
-  </si>
-  <si>
-    <t>Adeno-associated virus 6</t>
-  </si>
-  <si>
-    <t>AAV6</t>
-  </si>
-  <si>
-    <t>Adeno-associated virus 3B</t>
-  </si>
-  <si>
-    <t>AAV3B</t>
-  </si>
-  <si>
-    <t>AAV5</t>
-  </si>
-  <si>
-    <t>Adeno-associated virus 5</t>
-  </si>
-  <si>
-    <t>AAV9</t>
-  </si>
-  <si>
-    <t>Adeno-associated virus 9</t>
-  </si>
-  <si>
-    <t>Adeno-associated virus 11</t>
-  </si>
-  <si>
-    <t>AAV11</t>
-  </si>
-  <si>
-    <t>NHP-AAV-type2</t>
-  </si>
-  <si>
-    <t>NHP-AAV-type1</t>
-  </si>
-  <si>
-    <t>NHP Adeno-associated virus 11</t>
-  </si>
-  <si>
-    <t>NHP Adeno-associated virus type 2</t>
-  </si>
-  <si>
-    <t>NHP Adeno-associated virus type 1</t>
-  </si>
-  <si>
-    <t>NHP-AAV11</t>
-  </si>
-  <si>
-    <t>AAV4</t>
-  </si>
-  <si>
-    <t>Adeno-associated virus 4</t>
-  </si>
-  <si>
-    <t>AAV12</t>
-  </si>
-  <si>
-    <t>Adeno-associated virus 12</t>
-  </si>
-  <si>
-    <t>NHP Adeno-associated virus 6</t>
-  </si>
-  <si>
-    <t>NHP-AAV6</t>
-  </si>
-  <si>
-    <t>AAV10</t>
-  </si>
-  <si>
-    <t>AAV3</t>
-  </si>
-  <si>
-    <t>Adeno-associated virus 3</t>
-  </si>
-  <si>
-    <t>AAV1</t>
-  </si>
-  <si>
-    <t>Adeno-associated virus 1</t>
-  </si>
-  <si>
-    <t>AAV7</t>
-  </si>
-  <si>
-    <t>Adeno-associated virus 7</t>
-  </si>
-  <si>
-    <t>AAV8</t>
-  </si>
-  <si>
-    <t>Adeno-associated virus 8</t>
-  </si>
-  <si>
-    <t>Bearded dragon parvovirus strain 2014</t>
-  </si>
-  <si>
-    <t>BdrPV</t>
-  </si>
-  <si>
-    <t>Cairina moschata</t>
-  </si>
-  <si>
-    <t>Anser anser</t>
-  </si>
-  <si>
-    <t>Python regius</t>
-  </si>
-  <si>
-    <t>virus_clade</t>
-  </si>
-  <si>
-    <t>Reptile</t>
-  </si>
-  <si>
-    <t>Avian</t>
-  </si>
-  <si>
-    <t>AAV_primate</t>
-  </si>
-  <si>
-    <t>MF416383</t>
-  </si>
-  <si>
-    <t>MF416384</t>
-  </si>
-  <si>
-    <t>Mouse-AAV1</t>
-  </si>
-  <si>
-    <t>Mouse-AAV2</t>
-  </si>
-  <si>
-    <t>Mouse adeno associated virus 1</t>
-  </si>
-  <si>
-    <t>Mouse adeno associated virus 2</t>
-  </si>
-  <si>
-    <t>NC_004828</t>
-  </si>
-  <si>
-    <t>NC_005889</t>
-  </si>
-  <si>
-    <t>NC_006263</t>
-  </si>
-  <si>
-    <t>NC_014468</t>
-  </si>
-  <si>
-    <t>NC_038539</t>
-  </si>
-  <si>
-    <t>NC_040671</t>
-  </si>
-  <si>
-    <t>Avian adeno-associated virus ATCC VR-865</t>
-  </si>
-  <si>
-    <t>Bovine adeno-associated virus</t>
-  </si>
-  <si>
-    <t>Avian adeno-associated virus strain DA-1</t>
-  </si>
-  <si>
-    <t>Bat adeno-associated virus YNM</t>
-  </si>
-  <si>
-    <t>California sea lion adeno-associated virus 1</t>
-  </si>
-  <si>
-    <t>Avian adeno-associated virus isolate MHH-05-2015</t>
-  </si>
-  <si>
-    <t>AvAAV-da1</t>
-  </si>
-  <si>
-    <t>AvAAV-atcc</t>
-  </si>
-  <si>
-    <t>BAAV</t>
-  </si>
-  <si>
-    <t>AAV-bat</t>
-  </si>
-  <si>
-    <t>AvAAV-mhh</t>
-  </si>
-  <si>
-    <t>AAV-sealion</t>
+    <t>isolate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -399,13 +135,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF660066"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDEF3A8"/>
+        <fgColor rgb="FF002060"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1318,10 +1054,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="897">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2556,714 +2313,109 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="3" max="3" width="27.5" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" customWidth="1"/>
-    <col min="5" max="5" width="27.1640625" customWidth="1"/>
-    <col min="6" max="6" width="31.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="8" width="15.83203125" customWidth="1"/>
+    <col min="9" max="9" width="28.1640625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>20</v>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>24</v>
+      <c r="C2" s="1" t="b">
+        <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
+      <c r="B3" s="4"/>
+      <c r="C3" s="1" t="b">
+        <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>80</v>
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G31" s="2"/>
-    </row>
   </sheetData>
-  <sortState ref="A2:G106">
-    <sortCondition ref="E2:E106"/>
-    <sortCondition ref="F2:F106"/>
-    <sortCondition ref="D2:D106"/>
-  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Exclude modified sequences from alignment
</commit_message>
<xml_diff>
--- a/tabular/references/hhv-ncbi-refseqs-side-data.xlsx
+++ b/tabular/references/hhv-ncbi-refseqs-side-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/general/HHV6-GLUE/tabular/references/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/general/HHV6-GLUE/tabular/references/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2E667D-72EA-564F-9BE3-EA92E1F36011}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BAAC2F-413A-9949-8C6A-95049BECF353}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>clade</t>
-  </si>
-  <si>
-    <t>gb_lab_construct</t>
   </si>
   <si>
     <t>A1</t>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>isolate</t>
+  </si>
+  <si>
+    <t>lab_construct</t>
   </si>
 </sst>
 </file>
@@ -2317,7 +2317,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2345,22 +2345,22 @@
         <v>3</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -2368,26 +2368,26 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -2399,20 +2399,20 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>